<commit_message>
changed title on top readme
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
@@ -1456,9 +1456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>92880</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1467,8 +1467,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3357720" y="10725120"/>
-          <a:ext cx="6648480" cy="2258280"/>
+          <a:off x="3358440" y="10725480"/>
+          <a:ext cx="6648840" cy="2257560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,7 +1490,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1716,15 +1716,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -1732,8 +1732,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="41.84"/>
@@ -3905,70 +3905,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3984,7 +3984,7 @@
   </sheetPr>
   <dimension ref="B1:AD30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -3992,7 +3992,7 @@
       <selection pane="bottomRight" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5205,70 +5205,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5285,7 +5285,7 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
@@ -5293,7 +5293,7 @@
       <selection pane="bottomRight" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7574,70 +7574,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7653,11 +7653,11 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -7759,7 +7759,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Rb ROI and V+Sr standards
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Ce" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Lanthanides" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Version history" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="V+Sr" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Version history" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -130,8 +131,44 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="234">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -749,6 +786,57 @@
   </si>
   <si>
     <t xml:space="preserve">Nd(OH)3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-200  -30  -10 25 13k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 2 0.3 0.005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2O5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VanadylSulfate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOSO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrSulfate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrSO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrMolybdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrMoO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrHydroxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr(OH)2.8H2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrTitanate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrTiO3</t>
   </si>
   <si>
     <t xml:space="preserve">Current</t>
@@ -1456,9 +1544,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1467,8 +1555,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358440" y="10725480"/>
-          <a:ext cx="6648840" cy="2257560"/>
+          <a:off x="3358800" y="10725120"/>
+          <a:ext cx="6649200" cy="2257560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,7 +1578,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1716,15 +1804,15 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E46" activeCellId="0" sqref="E46"/>
+      <selection pane="bottomRight" activeCell="E46" activeCellId="1" sqref="H19:H22 E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -3905,70 +3993,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3985,14 +4073,14 @@
   <dimension ref="B1:AD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="P25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M19" activeCellId="0" sqref="M19"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="H19:H22 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -5205,70 +5293,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5290,10 +5378,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L53" activeCellId="0" sqref="L53"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="H19:H22 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7574,70 +7662,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7651,13 +7739,1301 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AD30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19:H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="19.7"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="str">
+        <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
+        <v>Version: 8</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="11"/>
+      <c r="Z2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="11"/>
+      <c r="Z3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="70.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB5" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC5" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="P6" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="44" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V6" s="45" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="W6" s="45" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="45" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="45" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="46" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
+      <c r="AD6" s="29"/>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="I7" s="53"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="54"/>
+      <c r="O7" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="P7" s="55"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="60"/>
+    </row>
+    <row r="8" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="I8" s="53"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N8" s="54"/>
+      <c r="O8" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="P8" s="55"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="59"/>
+      <c r="AA8" s="60"/>
+    </row>
+    <row r="9" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="48" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="L9" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" s="54"/>
+      <c r="O9" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="P9" s="55"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="57"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="59"/>
+      <c r="AA9" s="60"/>
+    </row>
+    <row r="10" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="53"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M10" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" s="54"/>
+      <c r="O10" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="P10" s="55"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="58"/>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="59"/>
+      <c r="AA10" s="60"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="48" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="55"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="59"/>
+      <c r="AA11" s="60"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="48" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="55"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="59"/>
+      <c r="AA12" s="60"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="48" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="55"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="59"/>
+      <c r="AA13" s="60"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="48" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="55"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="59"/>
+      <c r="AA14" s="60"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="48" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="55"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="59"/>
+      <c r="AA15" s="60"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="48" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="55"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="59"/>
+      <c r="AA16" s="60"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="48" t="n">
+        <v>23</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="55"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
+      <c r="Y17" s="58"/>
+      <c r="Z17" s="59"/>
+      <c r="AA17" s="60"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="48" t="n">
+        <v>24</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="55"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="60"/>
+    </row>
+    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I19" s="53"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="L19" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M19" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="54"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="55"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="60"/>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I20" s="53"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="L20" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M20" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="54"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="55"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
+      <c r="Y20" s="58"/>
+      <c r="Z20" s="59"/>
+      <c r="AA20" s="60"/>
+    </row>
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="48" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I21" s="53"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="L21" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M21" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N21" s="54"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="55"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="59"/>
+      <c r="AA21" s="60"/>
+    </row>
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I22" s="53"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="L22" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M22" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="N22" s="54"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="55"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+      <c r="Y22" s="58"/>
+      <c r="Z22" s="59"/>
+      <c r="AA22" s="60"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="48" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="55"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="59"/>
+      <c r="AA23" s="60"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="48" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="55"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="56"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+      <c r="Z24" s="59"/>
+      <c r="AA24" s="60"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="48" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="55"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="60"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="48" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="55"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+      <c r="Y26" s="58"/>
+      <c r="Z26" s="59"/>
+      <c r="AA26" s="60"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="48" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="55"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="59"/>
+      <c r="AA27" s="60"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="48" t="n">
+        <v>10</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="55"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="58"/>
+      <c r="Y28" s="58"/>
+      <c r="Z28" s="59"/>
+      <c r="AA28" s="60"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="48" t="n">
+        <v>23</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="55"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="58"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="58"/>
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="59"/>
+      <c r="AA29" s="60"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="48" t="n">
+        <v>24</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="55"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="58"/>
+      <c r="W30" s="58"/>
+      <c r="X30" s="58"/>
+      <c r="Y30" s="58"/>
+      <c r="Z30" s="59"/>
+      <c r="AA30" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:Z1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="U4:Z4"/>
+    <mergeCell ref="AA4:AC4"/>
+  </mergeCells>
+  <dataValidations count="14">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:Z30" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+      <formula1>"K,L3,L2,L1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A7:A30" type="whole">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C30" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6:B30" type="list">
+      <formula1>"Outer,Inner,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6:AC6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6:T30" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H19:H22 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -7665,12 +9041,12 @@
   <sheetData>
     <row r="1" s="64" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B2" s="64"/>
     </row>
@@ -7686,10 +9062,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7697,7 +9073,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7705,7 +9081,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7713,7 +9089,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7721,7 +9097,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,7 +9105,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7737,7 +9113,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7745,7 +9121,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7753,13 +9129,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
with beam, fix several bugs from shutdown work
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="242">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -794,19 +794,31 @@
     <t xml:space="preserve">VO2</t>
   </si>
   <si>
-    <t xml:space="preserve">10 2 0.3 0.05</t>
+    <t xml:space="preserve">Thermo Scientific; Vanadium (IV) oxide (99%); 022957.09; Lot T12H043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 2 0.3 0.05k</t>
   </si>
   <si>
     <t xml:space="preserve">V2O3</t>
   </si>
   <si>
+    <t xml:space="preserve">Sigma Aldrich; Vanadium (III) oxide; 463744-5G; Lot 0000089530</t>
+  </si>
+  <si>
     <t xml:space="preserve">V2O5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alfa Aesar; Vanadium (V) oxide (99.2%); 11093; Lot H03Q11</t>
   </si>
   <si>
     <t xml:space="preserve">VanadylSulfate</t>
   </si>
   <si>
     <t xml:space="preserve">VOSO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma Aldrich; Vanadium (IV) oxide sulfate hydrate (97%); 233706</t>
   </si>
   <si>
     <t xml:space="preserve">SrSulfate</t>
@@ -818,16 +830,25 @@
     <t xml:space="preserve">SrSO4</t>
   </si>
   <si>
+    <t xml:space="preserve">Celestine; Yate; UK</t>
+  </si>
+  <si>
     <t xml:space="preserve">SrMolybdate</t>
   </si>
   <si>
     <t xml:space="preserve">SrMoO4</t>
   </si>
   <si>
+    <t xml:space="preserve">Synthetic (Martin Stennett, University of Sheffield)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SrHydroxide</t>
   </si>
   <si>
     <t xml:space="preserve">Sr(OH)2.8H2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma Aldrich; 95%; 415219; Lot STBG0528V</t>
   </si>
   <si>
     <t xml:space="preserve">SrTitanate</t>
@@ -1250,7 +1271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="75">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1519,23 +1540,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1543,15 +1548,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1559,24 +1556,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1674,9 +1655,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1685,8 +1666,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358800" y="10725120"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3361320" y="10725120"/>
+          <a:ext cx="6650640" cy="2256480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1924,6 +1905,43 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>73080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1115280</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>94320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10722600"/>
+          <a:ext cx="3155400" cy="3272400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1933,24 +1951,24 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3358800" y="10725120"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3361320" y="6945120"/>
+          <a:ext cx="6650640" cy="2256480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2188,6 +2206,43 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1159200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>54000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6864480"/>
+          <a:ext cx="3199320" cy="1830960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2202,19 +2257,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1731960</xdr:colOff>
+      <xdr:colOff>1730880</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3391560" y="13656600"/>
-          <a:ext cx="6649200" cy="2257560"/>
+          <a:off x="3394080" y="13656600"/>
+          <a:ext cx="6650640" cy="2256480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2452,6 +2507,85 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158040</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>54360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1149840</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="158040" y="13629240"/>
+          <a:ext cx="3031920" cy="3115080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>324720</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>124920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7975800"/>
+          <a:ext cx="3591000" cy="2255040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2463,14 +2597,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="N25" activeCellId="0" sqref="B6:AD54"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2481,7 +2615,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
@@ -4743,10 +4877,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A31" activeCellId="1" sqref="B6:AD54 A31"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -34557,10 +34691,6 @@
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
-      <formula1>-150</formula1>
-      <formula2>150</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30 AW6:AZ30 CB6:CE30 DG6:DJ30 EL6:EO30 FQ6:FT30 GV6:GY30 IA6:ID30 JF6:JI30 KK6:KN30 LP6:LS30 MU6:MX30 NZ6:OC30 PE6:PH30 QJ6:QM30 RO6:RR30 ST6:SW30 TY6:UB30 VD6:VG30 WI6:WL30 XN6:XQ30 YS6:YV30 ZX6:AAA30 ABC6:ABF30 ACH6:ACK30 ADM6:ADP30 AER6:AEU30 AFW6:AFZ30 AHB6:AHE30 AIG6:AIJ30 AJL6:AJO30 AKQ6:AKT30 ALV6:ALY30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
@@ -34568,6 +34698,10 @@
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -34589,15 +34723,15 @@
   </sheetPr>
   <dimension ref="B1:AF54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="P7" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B6" activeCellId="0" sqref="B6:AD54"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -36964,15 +37098,15 @@
   </sheetPr>
   <dimension ref="B1:AE30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="6" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O7" activeCellId="0" sqref="B6:AD54"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -37130,88 +37264,87 @@
       <c r="C5" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="M5" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="N5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="68" t="s">
+      <c r="O5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="76" t="s">
+      <c r="P5" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="75" t="s">
+      <c r="Q5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="77" t="s">
+      <c r="R5" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="78" t="s">
+      <c r="S5" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="75" t="s">
+      <c r="T5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="79" t="s">
+      <c r="U5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="67" t="s">
+      <c r="V5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="69" t="s">
+      <c r="W5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="69" t="s">
+      <c r="X5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="69" t="s">
+      <c r="Y5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="69" t="s">
+      <c r="Z5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="73" t="s">
+      <c r="AA5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="71" t="s">
+      <c r="AB5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="80" t="s">
+      <c r="AC5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AD5" s="80" t="s">
+      <c r="AD5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AE5" s="81"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="30" t="s">
@@ -37293,9 +37426,9 @@
       <c r="AB6" s="47"/>
       <c r="AC6" s="42"/>
       <c r="AD6" s="42"/>
-      <c r="AE6" s="82"/>
+      <c r="AE6" s="72"/>
     </row>
-    <row r="7" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="47.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="48" t="n">
         <v>1</v>
       </c>
@@ -37311,7 +37444,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="83" t="s">
+      <c r="I7" s="73" t="s">
         <v>205</v>
       </c>
       <c r="J7" s="53"/>
@@ -37323,11 +37456,11 @@
         <v>129</v>
       </c>
       <c r="N7" s="61" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="O7" s="54"/>
       <c r="P7" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q7" s="55"/>
       <c r="T7" s="11"/>
@@ -37340,7 +37473,7 @@
       <c r="AA7" s="59"/>
       <c r="AB7" s="60"/>
     </row>
-    <row r="8" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="47.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="48" t="n">
         <v>2</v>
       </c>
@@ -37351,28 +37484,28 @@
         <v>5</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="73" t="s">
         <v>205</v>
       </c>
       <c r="J8" s="53"/>
       <c r="K8" s="48"/>
       <c r="L8" s="51" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M8" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N8" s="61" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="O8" s="54"/>
       <c r="P8" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q8" s="55"/>
       <c r="T8" s="11"/>
@@ -37396,28 +37529,28 @@
         <v>5</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="73" t="s">
         <v>205</v>
       </c>
       <c r="J9" s="53"/>
       <c r="K9" s="48"/>
       <c r="L9" s="29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M9" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N9" s="61" t="s">
-        <v>133</v>
+        <v>213</v>
       </c>
       <c r="O9" s="54"/>
       <c r="P9" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q9" s="55"/>
       <c r="T9" s="11"/>
@@ -37430,7 +37563,7 @@
       <c r="AA9" s="59"/>
       <c r="AB9" s="60"/>
     </row>
-    <row r="10" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="47.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="48" t="n">
         <v>4</v>
       </c>
@@ -37441,28 +37574,28 @@
         <v>5</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="83" t="s">
+      <c r="I10" s="73" t="s">
         <v>205</v>
       </c>
       <c r="J10" s="53"/>
       <c r="K10" s="48"/>
       <c r="L10" s="54" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="M10" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N10" s="61" t="s">
-        <v>133</v>
+        <v>216</v>
       </c>
       <c r="O10" s="54"/>
       <c r="P10" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q10" s="55"/>
       <c r="T10" s="11"/>
@@ -37489,7 +37622,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="83"/>
+      <c r="I11" s="73"/>
       <c r="J11" s="53"/>
       <c r="K11" s="48"/>
       <c r="L11" s="54"/>
@@ -37522,7 +37655,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="83"/>
+      <c r="I12" s="73"/>
       <c r="J12" s="53"/>
       <c r="K12" s="48"/>
       <c r="L12" s="54"/>
@@ -37555,7 +37688,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="83"/>
+      <c r="I13" s="73"/>
       <c r="J13" s="53"/>
       <c r="K13" s="48"/>
       <c r="L13" s="54"/>
@@ -37588,7 +37721,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="83"/>
+      <c r="I14" s="73"/>
       <c r="J14" s="53"/>
       <c r="K14" s="48"/>
       <c r="L14" s="54"/>
@@ -37621,7 +37754,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="83"/>
+      <c r="I15" s="73"/>
       <c r="J15" s="53"/>
       <c r="K15" s="48"/>
       <c r="L15" s="54"/>
@@ -37654,7 +37787,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="83"/>
+      <c r="I16" s="73"/>
       <c r="J16" s="53"/>
       <c r="K16" s="48"/>
       <c r="L16" s="54"/>
@@ -37687,7 +37820,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="83"/>
+      <c r="I17" s="73"/>
       <c r="J17" s="53"/>
       <c r="K17" s="48"/>
       <c r="L17" s="54"/>
@@ -37720,7 +37853,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="83"/>
+      <c r="I18" s="73"/>
       <c r="J18" s="53"/>
       <c r="K18" s="48"/>
       <c r="L18" s="54"/>
@@ -37739,7 +37872,7 @@
       <c r="AA18" s="59"/>
       <c r="AB18" s="60"/>
     </row>
-    <row r="19" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="48" t="n">
         <v>1</v>
       </c>
@@ -37750,24 +37883,24 @@
         <v>5</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="83" t="s">
-        <v>214</v>
+      <c r="I19" s="73" t="s">
+        <v>218</v>
       </c>
       <c r="J19" s="53"/>
       <c r="K19" s="48"/>
       <c r="L19" s="51" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="M19" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N19" s="61" t="s">
-        <v>133</v>
+        <v>220</v>
       </c>
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
@@ -37782,7 +37915,7 @@
       <c r="AA19" s="59"/>
       <c r="AB19" s="60"/>
     </row>
-    <row r="20" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="48" t="n">
         <v>2</v>
       </c>
@@ -37793,24 +37926,24 @@
         <v>5</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="83" t="s">
-        <v>214</v>
+      <c r="I20" s="73" t="s">
+        <v>218</v>
       </c>
       <c r="J20" s="53"/>
       <c r="K20" s="48"/>
       <c r="L20" s="51" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="M20" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N20" s="61" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="O20" s="54"/>
       <c r="P20" s="29"/>
@@ -37836,24 +37969,24 @@
         <v>5</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="83" t="s">
-        <v>214</v>
+      <c r="I21" s="73" t="s">
+        <v>218</v>
       </c>
       <c r="J21" s="53"/>
       <c r="K21" s="48"/>
       <c r="L21" s="29" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="M21" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N21" s="61" t="s">
-        <v>133</v>
+        <v>226</v>
       </c>
       <c r="O21" s="54"/>
       <c r="P21" s="29"/>
@@ -37879,24 +38012,24 @@
         <v>3</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="83" t="s">
-        <v>214</v>
+      <c r="I22" s="73" t="s">
+        <v>218</v>
       </c>
       <c r="J22" s="53"/>
       <c r="K22" s="48"/>
       <c r="L22" s="29" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="M22" s="51" t="s">
         <v>129</v>
       </c>
       <c r="N22" s="61" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="O22" s="54"/>
       <c r="P22" s="29"/>
@@ -37911,7 +38044,7 @@
       <c r="AA22" s="59"/>
       <c r="AB22" s="60"/>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="n">
         <v>5</v>
       </c>
@@ -37925,7 +38058,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="83"/>
+      <c r="I23" s="73"/>
       <c r="J23" s="53"/>
       <c r="K23" s="48"/>
       <c r="L23" s="29"/>
@@ -37958,7 +38091,7 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="83"/>
+      <c r="I24" s="73"/>
       <c r="J24" s="53"/>
       <c r="K24" s="48"/>
       <c r="L24" s="29"/>
@@ -37991,7 +38124,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="83"/>
+      <c r="I25" s="73"/>
       <c r="J25" s="53"/>
       <c r="K25" s="48"/>
       <c r="L25" s="29"/>
@@ -38024,7 +38157,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="83"/>
+      <c r="I26" s="73"/>
       <c r="J26" s="53"/>
       <c r="K26" s="48"/>
       <c r="L26" s="29"/>
@@ -38057,7 +38190,7 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="83"/>
+      <c r="I27" s="73"/>
       <c r="J27" s="53"/>
       <c r="K27" s="48"/>
       <c r="L27" s="29"/>
@@ -38090,7 +38223,7 @@
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="83"/>
+      <c r="I28" s="73"/>
       <c r="J28" s="53"/>
       <c r="K28" s="48"/>
       <c r="L28" s="54"/>
@@ -38123,7 +38256,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="83"/>
+      <c r="I29" s="73"/>
       <c r="J29" s="53"/>
       <c r="K29" s="48"/>
       <c r="L29" s="54"/>
@@ -38156,7 +38289,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="83"/>
+      <c r="I30" s="73"/>
       <c r="J30" s="53"/>
       <c r="K30" s="48"/>
       <c r="L30" s="54"/>
@@ -38192,21 +38325,65 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="22">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA6" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+      <formula1>"K,L3,L2,L1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2" type="list">
       <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
+      <formula1>"Outer,Inner,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
-      <formula1>1</formula1>
-      <formula2>24</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
@@ -38219,14 +38396,6 @@
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
@@ -38244,42 +38413,6 @@
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
-      <formula1>"Outer,Inner,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
-      <formula1>"K,L3,L2,L1"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6" type="list">
-      <formula1>"unfocused,focused"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA6" type="list">
-      <formula1>"True,False"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
-    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -38288,7 +38421,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -38300,42 +38434,42 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="B6:AD54 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>
-    <row r="1" s="84" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="74" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="84"/>
+        <v>230</v>
+      </c>
+      <c r="B2" s="74"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="74"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="28"/>
-      <c r="B4" s="84"/>
+      <c r="B4" s="74"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="84" t="s">
-        <v>224</v>
+        <v>230</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38343,7 +38477,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38351,7 +38485,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38359,7 +38493,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38367,7 +38501,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38375,7 +38509,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38383,7 +38517,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38391,7 +38525,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38399,7 +38533,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38407,7 +38541,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38415,7 +38549,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ROIs, standards spreadsheet, some usability tweaks
* downgrade warning about mode B to not require interaction
* fix some bugs from adding finalize_wrapper to change_edge
* notice a spreadsheet with an edge out of range
* put Sc in Ir slot on ref wheel
* fix plotting bug when measuring an element not on ref wheel
* add many L line positions to rois.json
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
@@ -338,7 +338,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="435">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -1234,12 +1234,12 @@
     <t xml:space="preserve">Ca2ZnSi2O7</t>
   </si>
   <si>
+    <t xml:space="preserve">Ti</t>
+  </si>
+  <si>
     <t xml:space="preserve">TitaniumFoil</t>
   </si>
   <si>
-    <t xml:space="preserve">Ti</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ti foil</t>
   </si>
   <si>
@@ -1255,6 +1255,9 @@
     <t xml:space="preserve">CsNO3</t>
   </si>
   <si>
+    <t xml:space="preserve">-200  -30  -10 25  335</t>
+  </si>
+  <si>
     <t xml:space="preserve">BariumSomething</t>
   </si>
   <si>
@@ -1273,12 +1276,18 @@
     <t xml:space="preserve">La(OH)3</t>
   </si>
   <si>
+    <t xml:space="preserve">-200  -30  -10 25  390</t>
+  </si>
+  <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
     <t xml:space="preserve">CeriumDioxide</t>
   </si>
   <si>
+    <t xml:space="preserve">-200  -30  -10 25  420</t>
+  </si>
+  <si>
     <t xml:space="preserve">PraseodymiumOxide</t>
   </si>
   <si>
@@ -1553,6 +1562,9 @@
   </si>
   <si>
     <t xml:space="preserve">YttriumOxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">Y2O3</t>
@@ -2859,9 +2871,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>54720</xdr:rowOff>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2870,8 +2882,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3366360" y="10725120"/>
-          <a:ext cx="6653880" cy="2254680"/>
+          <a:off x="3367080" y="10725120"/>
+          <a:ext cx="6653880" cy="2254320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3118,9 +3130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1113480</xdr:colOff>
+      <xdr:colOff>1113120</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3134,7 +3146,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10722600"/>
-          <a:ext cx="3158640" cy="3270600"/>
+          <a:ext cx="3159000" cy="3270240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3160,9 +3172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>67680</xdr:colOff>
+      <xdr:colOff>67320</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3171,8 +3183,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3344400" y="7834680"/>
-          <a:ext cx="6653880" cy="2254680"/>
+          <a:off x="3345120" y="7834680"/>
+          <a:ext cx="6653880" cy="2254320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3419,9 +3431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1157400</xdr:colOff>
+      <xdr:colOff>1157040</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3435,7 +3447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7716240"/>
-          <a:ext cx="3202560" cy="1829160"/>
+          <a:ext cx="3202920" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3461,9 +3473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1729080</xdr:colOff>
+      <xdr:colOff>1728720</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3472,8 +3484,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3399120" y="13656600"/>
-          <a:ext cx="6653880" cy="2254680"/>
+          <a:off x="3399840" y="13656600"/>
+          <a:ext cx="6654240" cy="2254320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3720,9 +3732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1148040</xdr:colOff>
+      <xdr:colOff>1147680</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3736,7 +3748,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="158040" y="13629240"/>
-          <a:ext cx="3035160" cy="3113280"/>
+          <a:ext cx="3035520" cy="3112920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3762,9 +3774,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>322920</xdr:colOff>
+      <xdr:colOff>322560</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3778,7 +3790,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7947360"/>
-          <a:ext cx="3594960" cy="2253240"/>
+          <a:ext cx="3595680" cy="2252880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3804,9 +3816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1866240</xdr:colOff>
+      <xdr:colOff>1865880</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3816,7 +3828,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6649200" cy="2254680"/>
+          <a:ext cx="6648840" cy="2254320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4063,9 +4075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1113480</xdr:colOff>
+      <xdr:colOff>1113120</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4079,7 +4091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10262880"/>
-          <a:ext cx="3154320" cy="3270600"/>
+          <a:ext cx="3153960" cy="3270240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4105,9 +4117,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1866240</xdr:colOff>
+      <xdr:colOff>1865880</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4117,7 +4129,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6649200" cy="2254680"/>
+          <a:ext cx="6648840" cy="2254320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4364,9 +4376,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1113480</xdr:colOff>
+      <xdr:colOff>1113120</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4380,7 +4392,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10995120"/>
-          <a:ext cx="3154320" cy="3270600"/>
+          <a:ext cx="3153960" cy="3270240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4416,7 +4428,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -6708,7 +6720,7 @@
       <selection pane="bottomRight" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -8042,7 +8054,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -10417,7 +10429,7 @@
       <selection pane="bottomRight" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -11758,7 +11770,7 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
@@ -15996,11 +16008,11 @@
   </sheetPr>
   <dimension ref="B1:AD80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -16276,10 +16288,10 @@
         <v>48</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>49</v>
+        <v>225</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>51</v>
@@ -16348,13 +16360,13 @@
         <v>5</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="150" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J7" s="151" t="s">
         <v>51</v>
@@ -16382,7 +16394,7 @@
       <c r="AA7" s="59"/>
       <c r="AB7" s="60"/>
     </row>
-    <row r="8" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="48" t="n">
         <v>1</v>
       </c>
@@ -16414,7 +16426,9 @@
       <c r="N8" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="O8" s="54"/>
+      <c r="O8" s="64" t="s">
+        <v>305</v>
+      </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="55"/>
       <c r="T8" s="11"/>
@@ -16438,20 +16452,20 @@
         <v>3</v>
       </c>
       <c r="E9" s="156" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F9" s="153"/>
       <c r="G9" s="153"/>
       <c r="H9" s="153"/>
       <c r="I9" s="157" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J9" s="158" t="s">
         <v>135</v>
       </c>
       <c r="K9" s="153"/>
       <c r="L9" s="159" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M9" s="156"/>
       <c r="N9" s="160"/>
@@ -16477,7 +16491,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -16511,7 +16525,7 @@
       <c r="AA10" s="59"/>
       <c r="AB10" s="60"/>
     </row>
-    <row r="11" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="48" t="n">
         <v>1</v>
       </c>
@@ -16522,7 +16536,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -16535,7 +16549,7 @@
       </c>
       <c r="K11" s="48"/>
       <c r="L11" s="54" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M11" s="51" t="s">
         <v>77</v>
@@ -16543,7 +16557,9 @@
       <c r="N11" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="O11" s="54"/>
+      <c r="O11" s="64" t="s">
+        <v>312</v>
+      </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="55"/>
       <c r="T11" s="11"/>
@@ -16576,7 +16592,7 @@
         <v>303</v>
       </c>
       <c r="J12" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K12" s="48"/>
       <c r="L12" s="54" t="s">
@@ -16601,7 +16617,7 @@
       <c r="AA12" s="59"/>
       <c r="AB12" s="60"/>
     </row>
-    <row r="13" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="48" t="n">
         <v>1</v>
       </c>
@@ -16612,7 +16628,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -16633,7 +16649,9 @@
       <c r="N13" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="O13" s="54"/>
+      <c r="O13" s="64" t="s">
+        <v>315</v>
+      </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="55"/>
       <c r="T13" s="11"/>
@@ -16657,7 +16675,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -16670,7 +16688,7 @@
       </c>
       <c r="K14" s="48"/>
       <c r="L14" s="54" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="M14" s="51" t="s">
         <v>77</v>
@@ -16704,20 +16722,20 @@
         <v>5</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="150" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="J15" s="151" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="54" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="M15" s="51" t="s">
         <v>279</v>
@@ -16749,20 +16767,20 @@
         <v>3</v>
       </c>
       <c r="E16" s="156" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F16" s="153"/>
       <c r="G16" s="153"/>
       <c r="H16" s="153"/>
       <c r="I16" s="157" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J16" s="158" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K16" s="153"/>
       <c r="L16" s="159" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M16" s="156"/>
       <c r="N16" s="160"/>
@@ -16788,7 +16806,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -16801,7 +16819,7 @@
       </c>
       <c r="K17" s="48"/>
       <c r="L17" s="54" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="M17" s="51" t="s">
         <v>77</v>
@@ -16835,7 +16853,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -16844,11 +16862,11 @@
         <v>149</v>
       </c>
       <c r="J18" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="54" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M18" s="51" t="s">
         <v>77</v>
@@ -16880,7 +16898,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -16893,13 +16911,13 @@
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="54" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="M19" s="51" t="s">
         <v>225</v>
       </c>
       <c r="N19" s="143" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
@@ -16925,7 +16943,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -16934,7 +16952,7 @@
         <v>134</v>
       </c>
       <c r="J20" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="54" t="s">
@@ -16970,7 +16988,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="51" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -16983,7 +17001,7 @@
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="54" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="M21" s="51" t="s">
         <v>77</v>
@@ -17017,7 +17035,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -17026,11 +17044,11 @@
         <v>170</v>
       </c>
       <c r="J22" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="54" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="M22" s="51" t="s">
         <v>77</v>
@@ -17062,7 +17080,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -17075,7 +17093,7 @@
       </c>
       <c r="K23" s="48"/>
       <c r="L23" s="54" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="M23" s="51" t="s">
         <v>77</v>
@@ -17109,7 +17127,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="51" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -17122,7 +17140,7 @@
       </c>
       <c r="K24" s="48"/>
       <c r="L24" s="54" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="M24" s="51" t="s">
         <v>279</v>
@@ -17154,7 +17172,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -17163,11 +17181,11 @@
         <v>181</v>
       </c>
       <c r="J25" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K25" s="48"/>
       <c r="L25" s="54" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="M25" s="51" t="s">
         <v>77</v>
@@ -17199,7 +17217,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -17212,7 +17230,7 @@
       </c>
       <c r="K26" s="48"/>
       <c r="L26" s="54" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M26" s="51" t="s">
         <v>77</v>
@@ -17246,7 +17264,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -17259,7 +17277,7 @@
       </c>
       <c r="K27" s="48"/>
       <c r="L27" s="54" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="M27" s="51" t="s">
         <v>77</v>
@@ -17293,20 +17311,20 @@
         <v>5</v>
       </c>
       <c r="E28" s="51" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="150" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="J28" s="151" t="s">
         <v>51</v>
       </c>
       <c r="K28" s="48"/>
       <c r="L28" s="54" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="M28" s="51" t="s">
         <v>279</v>
@@ -17338,7 +17356,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -17347,11 +17365,11 @@
         <v>151</v>
       </c>
       <c r="J29" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K29" s="48"/>
       <c r="L29" s="54" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="M29" s="51" t="s">
         <v>77</v>
@@ -17383,7 +17401,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -17396,7 +17414,7 @@
       </c>
       <c r="K30" s="48"/>
       <c r="L30" s="54" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="M30" s="51" t="s">
         <v>77</v>
@@ -17430,7 +17448,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -17439,11 +17457,11 @@
         <v>155</v>
       </c>
       <c r="J31" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K31" s="48"/>
       <c r="L31" s="54" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="M31" s="51" t="s">
         <v>77</v>
@@ -17475,7 +17493,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="51" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
@@ -17488,7 +17506,7 @@
       </c>
       <c r="K32" s="48"/>
       <c r="L32" s="54" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="M32" s="51" t="s">
         <v>77</v>
@@ -17522,20 +17540,20 @@
         <v>5</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="150" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="J33" s="151" t="s">
         <v>51</v>
       </c>
       <c r="K33" s="48"/>
       <c r="L33" s="54" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="M33" s="51" t="s">
         <v>279</v>
@@ -17567,7 +17585,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="51" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
@@ -17612,7 +17630,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="51" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
@@ -17621,11 +17639,11 @@
         <v>165</v>
       </c>
       <c r="J35" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K35" s="48"/>
       <c r="L35" s="54" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M35" s="51" t="s">
         <v>77</v>
@@ -17657,7 +17675,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="51" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -17670,7 +17688,7 @@
       </c>
       <c r="K36" s="48"/>
       <c r="L36" s="54" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="M36" s="51" t="s">
         <v>77</v>
@@ -17702,7 +17720,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -17711,11 +17729,11 @@
         <v>187</v>
       </c>
       <c r="J37" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K37" s="48"/>
       <c r="L37" s="54" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="M37" s="51" t="s">
         <v>77</v>
@@ -17747,7 +17765,7 @@
         <v>5</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
@@ -17792,7 +17810,7 @@
         <v>5</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
@@ -17805,7 +17823,7 @@
       </c>
       <c r="K39" s="48"/>
       <c r="L39" s="54" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="M39" s="51" t="s">
         <v>279</v>
@@ -17837,7 +17855,7 @@
         <v>5</v>
       </c>
       <c r="E40" s="51" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -17846,11 +17864,11 @@
         <v>190</v>
       </c>
       <c r="J40" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K40" s="48"/>
       <c r="L40" s="54" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="M40" s="51" t="s">
         <v>77</v>
@@ -17882,7 +17900,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="51" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -17895,7 +17913,7 @@
       </c>
       <c r="K41" s="48"/>
       <c r="L41" s="54" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="M41" s="51" t="s">
         <v>77</v>
@@ -17927,7 +17945,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="51" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -17936,11 +17954,11 @@
         <v>193</v>
       </c>
       <c r="J42" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K42" s="48"/>
       <c r="L42" s="54" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="M42" s="51" t="s">
         <v>77</v>
@@ -17972,20 +17990,20 @@
         <v>5</v>
       </c>
       <c r="E43" s="51" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="150" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="J43" s="151" t="s">
         <v>135</v>
       </c>
       <c r="K43" s="48"/>
       <c r="L43" s="54" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="M43" s="51" t="s">
         <v>77</v>
@@ -18017,7 +18035,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="51" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -18030,7 +18048,7 @@
       </c>
       <c r="K44" s="48"/>
       <c r="L44" s="54" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="M44" s="51" t="s">
         <v>279</v>
@@ -18062,7 +18080,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="51" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -18071,7 +18089,7 @@
         <v>159</v>
       </c>
       <c r="J45" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K45" s="48"/>
       <c r="L45" s="54" t="s">
@@ -18107,20 +18125,20 @@
         <v>5</v>
       </c>
       <c r="E46" s="51" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="150" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="J46" s="151" t="s">
         <v>135</v>
       </c>
       <c r="K46" s="48"/>
       <c r="L46" s="54" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="M46" s="51" t="s">
         <v>77</v>
@@ -18152,7 +18170,7 @@
         <v>5</v>
       </c>
       <c r="E47" s="51" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -18161,11 +18179,11 @@
         <v>197</v>
       </c>
       <c r="J47" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K47" s="48"/>
       <c r="L47" s="54" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="M47" s="51" t="s">
         <v>77</v>
@@ -18197,20 +18215,20 @@
         <v>5</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="150" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="J48" s="151" t="s">
         <v>135</v>
       </c>
       <c r="K48" s="48"/>
       <c r="L48" s="54" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M48" s="51" t="s">
         <v>77</v>
@@ -18242,20 +18260,20 @@
         <v>5</v>
       </c>
       <c r="E49" s="51" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="150" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="J49" s="151" t="s">
         <v>51</v>
       </c>
       <c r="K49" s="48"/>
       <c r="L49" s="54" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="M49" s="51" t="s">
         <v>77</v>
@@ -18287,7 +18305,7 @@
         <v>5</v>
       </c>
       <c r="E50" s="51" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -18296,7 +18314,7 @@
         <v>162</v>
       </c>
       <c r="J50" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K50" s="48"/>
       <c r="L50" s="54" t="s">
@@ -18332,20 +18350,20 @@
         <v>5</v>
       </c>
       <c r="E51" s="51" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
       <c r="I51" s="150" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="J51" s="151" t="s">
         <v>135</v>
       </c>
       <c r="K51" s="48"/>
       <c r="L51" s="54" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="M51" s="143" t="s">
         <v>54</v>
@@ -18375,7 +18393,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -18384,11 +18402,11 @@
         <v>201</v>
       </c>
       <c r="J52" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K52" s="48"/>
       <c r="L52" s="54" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="M52" s="51" t="s">
         <v>77</v>
@@ -18420,20 +18438,20 @@
         <v>3</v>
       </c>
       <c r="E53" s="156" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="F53" s="153"/>
       <c r="G53" s="153"/>
       <c r="H53" s="153"/>
       <c r="I53" s="157" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="J53" s="158" t="s">
         <v>135</v>
       </c>
       <c r="K53" s="153"/>
       <c r="L53" s="159" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="M53" s="161"/>
       <c r="N53" s="160"/>
@@ -18459,20 +18477,20 @@
         <v>5</v>
       </c>
       <c r="E54" s="51" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="150" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="J54" s="151" t="s">
         <v>51</v>
       </c>
       <c r="K54" s="48"/>
       <c r="L54" s="54" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="M54" s="51" t="s">
         <v>77</v>
@@ -18504,16 +18522,16 @@
         <v>3</v>
       </c>
       <c r="E55" s="156" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="I55" s="157" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="J55" s="158" t="s">
         <v>135</v>
       </c>
       <c r="L55" s="152" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="N55" s="163"/>
       <c r="V55" s="164"/>
@@ -18534,16 +18552,16 @@
         <v>5</v>
       </c>
       <c r="E56" s="51" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="I56" s="150" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="J56" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L56" s="54" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="M56" s="51" t="s">
         <v>77</v>
@@ -18563,16 +18581,16 @@
         <v>5</v>
       </c>
       <c r="E57" s="51" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I57" s="150" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="J57" s="151" t="s">
         <v>135</v>
       </c>
       <c r="L57" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="M57" s="51" t="s">
         <v>279</v>
@@ -18592,16 +18610,16 @@
         <v>5</v>
       </c>
       <c r="E58" s="51" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I58" s="150" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="J58" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L58" s="54" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="M58" s="51" t="s">
         <v>77</v>
@@ -18621,16 +18639,16 @@
         <v>5</v>
       </c>
       <c r="E59" s="51" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I59" s="150" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="J59" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="M59" s="143" t="s">
         <v>54</v>
@@ -18647,16 +18665,16 @@
         <v>5</v>
       </c>
       <c r="E60" s="51" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I60" s="150" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="J60" s="151" t="s">
         <v>135</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="M60" s="51" t="s">
         <v>279</v>
@@ -18676,16 +18694,16 @@
         <v>5</v>
       </c>
       <c r="E61" s="51" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="I61" s="150" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="J61" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L61" s="54" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M61" s="51" t="s">
         <v>77</v>
@@ -18705,16 +18723,16 @@
         <v>5</v>
       </c>
       <c r="E62" s="51" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="I62" s="150" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="J62" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L62" s="54" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="M62" s="143" t="s">
         <v>54</v>
@@ -18731,16 +18749,16 @@
         <v>5</v>
       </c>
       <c r="E63" s="51" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I63" s="150" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="J63" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L63" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="M63" s="51" t="s">
         <v>77</v>
@@ -18757,19 +18775,19 @@
         <v>46</v>
       </c>
       <c r="D64" s="155" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" s="156" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="I64" s="157" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="J64" s="158" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L64" s="159" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="N64" s="163"/>
       <c r="V64" s="164"/>
@@ -18790,16 +18808,16 @@
         <v>5</v>
       </c>
       <c r="E65" s="51" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="I65" s="150" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="J65" s="151" t="s">
         <v>135</v>
       </c>
       <c r="L65" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="M65" s="51" t="s">
         <v>279</v>
@@ -18819,16 +18837,16 @@
         <v>5</v>
       </c>
       <c r="E66" s="51" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="I66" s="150" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="J66" s="151" t="s">
         <v>135</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="M66" s="143" t="s">
         <v>54</v>
@@ -18843,19 +18861,19 @@
         <v>46</v>
       </c>
       <c r="D67" s="155" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E67" s="156" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="I67" s="157" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="J67" s="158" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L67" s="152" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="N67" s="163"/>
       <c r="V67" s="164"/>
@@ -18876,22 +18894,22 @@
         <v>5</v>
       </c>
       <c r="E68" s="51" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="I68" s="150" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="J68" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L68" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="M68" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="N68" s="61" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18905,16 +18923,16 @@
         <v>5</v>
       </c>
       <c r="E69" s="51" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I69" s="150" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="J69" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L69" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="M69" s="51" t="s">
         <v>279</v>
@@ -18931,16 +18949,16 @@
         <v>5</v>
       </c>
       <c r="E70" s="51" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I70" s="150" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="J70" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="M70" s="51" t="s">
         <v>279</v>
@@ -18957,16 +18975,16 @@
         <v>5</v>
       </c>
       <c r="E71" s="51" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="I71" s="150" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="J71" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="M71" s="51" t="s">
         <v>77</v>
@@ -18986,16 +19004,16 @@
         <v>5</v>
       </c>
       <c r="E72" s="51" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="I72" s="150" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="J72" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="M72" s="51" t="s">
         <v>279</v>
@@ -19015,7 +19033,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="51" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="I73" s="150" t="s">
         <v>230</v>
@@ -19044,16 +19062,16 @@
         <v>5</v>
       </c>
       <c r="E74" s="51" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="I74" s="150" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="J74" s="151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L74" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="M74" s="143" t="s">
         <v>54</v>
@@ -19070,16 +19088,16 @@
         <v>5</v>
       </c>
       <c r="E75" s="51" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="I75" s="150" t="s">
-        <v>162</v>
+        <v>408</v>
       </c>
       <c r="J75" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="M75" s="51" t="s">
         <v>77</v>
@@ -19099,16 +19117,16 @@
         <v>5</v>
       </c>
       <c r="E76" s="51" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="I76" s="150" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="J76" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L76" s="0" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="M76" s="51" t="s">
         <v>279</v>
@@ -19128,16 +19146,16 @@
         <v>5</v>
       </c>
       <c r="E77" s="51" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="I77" s="150" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="J77" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L77" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="M77" s="51" t="s">
         <v>279</v>
@@ -19157,16 +19175,16 @@
         <v>5</v>
       </c>
       <c r="E78" s="51" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I78" s="150" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="J78" s="151" t="s">
         <v>51</v>
       </c>
       <c r="L78" s="0" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="M78" s="51" t="s">
         <v>279</v>
@@ -19186,16 +19204,16 @@
         <v>3</v>
       </c>
       <c r="E79" s="169" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="I79" s="170" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="J79" s="171" t="s">
         <v>51</v>
       </c>
       <c r="L79" s="165" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="M79" s="172" t="s">
         <v>77</v>
@@ -19229,32 +19247,8 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B79" type="whole">
-      <formula1>1</formula1>
-      <formula2>24</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C79" type="list">
-      <formula1>"Outer,Inner,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D79" type="list">
-      <formula1>"Yes,No"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I79" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+      <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J79" type="list">
@@ -19265,29 +19259,53 @@
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B79" type="whole">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D79" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I79" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C79" type="list">
+      <formula1>"Outer,Inner,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
-      <formula1>"True,False"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -19312,7 +19330,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -19320,12 +19338,12 @@
   <sheetData>
     <row r="1" s="176" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B2" s="176"/>
     </row>
@@ -19341,10 +19359,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B5" s="176" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19352,7 +19370,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19360,7 +19378,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19368,7 +19386,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19376,7 +19394,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19384,7 +19402,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19392,7 +19410,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19400,7 +19418,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19408,7 +19426,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19416,7 +19434,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19424,7 +19442,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up standards spreadsheet a bit
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -72,7 +72,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -108,7 +108,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -200,7 +200,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -236,7 +236,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -272,7 +272,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -308,7 +308,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -344,7 +344,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -380,7 +380,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -416,7 +416,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -452,7 +452,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -3226,9 +3226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>88920</xdr:colOff>
+      <xdr:colOff>88560</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3237,8 +3237,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3367800" y="10725120"/>
-          <a:ext cx="6654240" cy="2253960"/>
+          <a:off x="3369240" y="10725120"/>
+          <a:ext cx="6655320" cy="2253960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3260,7 +3260,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -3485,9 +3485,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
+      <xdr:colOff>1112400</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3501,12 +3501,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10722600"/>
-          <a:ext cx="3159360" cy="3269880"/>
+          <a:ext cx="3160440" cy="3269520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -3527,9 +3527,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>66960</xdr:colOff>
+      <xdr:colOff>66600</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3538,8 +3538,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3345840" y="7834680"/>
-          <a:ext cx="6654240" cy="2253960"/>
+          <a:off x="3347280" y="7834680"/>
+          <a:ext cx="6655320" cy="2253960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3561,7 +3561,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -3786,9 +3786,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1156680</xdr:colOff>
+      <xdr:colOff>1156320</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3802,12 +3802,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7716240"/>
-          <a:ext cx="3203280" cy="1828440"/>
+          <a:ext cx="3204360" cy="1828080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -3828,9 +3828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1728360</xdr:colOff>
+      <xdr:colOff>1728000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3839,8 +3839,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3400560" y="13656600"/>
-          <a:ext cx="6654240" cy="2253960"/>
+          <a:off x="3402000" y="13656600"/>
+          <a:ext cx="6655320" cy="2253600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3862,7 +3862,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -4087,9 +4087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1147320</xdr:colOff>
+      <xdr:colOff>1146960</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4103,12 +4103,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="158040" y="13629240"/>
-          <a:ext cx="3035880" cy="3112560"/>
+          <a:ext cx="3036960" cy="3112560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -4129,9 +4129,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>322200</xdr:colOff>
+      <xdr:colOff>321840</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4145,12 +4145,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7947360"/>
-          <a:ext cx="3596760" cy="2252520"/>
+          <a:ext cx="3597840" cy="2252520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -4171,9 +4171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865520</xdr:colOff>
+      <xdr:colOff>1865160</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4183,7 +4183,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648480" cy="2253960"/>
+          <a:ext cx="6648120" cy="2253600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4205,7 +4205,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -4421,43 +4421,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="10262880"/>
-          <a:ext cx="3153600" cy="3269880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4472,19 +4435,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865520</xdr:colOff>
+      <xdr:colOff>1865160</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648480" cy="2253960"/>
+          <a:ext cx="6648120" cy="2253600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4506,7 +4469,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -4722,43 +4685,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5659920"/>
-          <a:ext cx="3153600" cy="3269880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4773,19 +4699,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865520</xdr:colOff>
+      <xdr:colOff>1865160</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
+        <xdr:cNvPr id="9" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648480" cy="2253960"/>
+          <a:ext cx="6648120" cy="2253600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4807,7 +4733,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -5023,43 +4949,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5659920"/>
-          <a:ext cx="3153600" cy="3269880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5074,19 +4963,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865520</xdr:colOff>
+      <xdr:colOff>1865160</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvPr id="10" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648480" cy="2253960"/>
+          <a:off x="3362040" y="10725480"/>
+          <a:ext cx="6648120" cy="2253600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5108,7 +4997,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -5333,13 +5222,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
+      <xdr:colOff>1112400</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 1" descr=""/>
+        <xdr:cNvPr id="11" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5348,314 +5237,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="11065320"/>
-          <a:ext cx="3153600" cy="3269880"/>
+          <a:off x="0" y="11065680"/>
+          <a:ext cx="3153240" cy="3269160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1321200</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1607040</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648480" cy="2253960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="73080">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Instructions:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>2. Default values for all parameters go in line 6</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Specify detector position in column U, blank means to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>not move</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t> the detector </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Do not add rows above row 7</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>7. Do not add columns before column AE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112760</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="10013040"/>
-          <a:ext cx="3153600" cy="3269880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -5686,7 +5274,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7886,74 +7474,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7970,12 +7558,12 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10037,80 +9625,79 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J19 J24:J25 J28:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J19 J24:J25 J28:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K25 K28:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K25 K28:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F25 F28:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F25 F28:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H25 H28:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H25 H28:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I25 I28:I54" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I25 I28:I54" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10125,7 +9712,7 @@
       <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -10181,7 +9768,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="e">
         <f aca="false">_xlfn.CONCAT("Version: ",'[1]Version history'!A3)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -13360,70 +12947,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J79" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J79" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B79" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B79" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D79" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D79" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I79" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I79" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C79" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C79" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -13443,7 +13030,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -13561,7 +13148,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -13584,7 +13171,7 @@
       <selection pane="bottomRight" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -14826,74 +14413,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -14918,7 +14505,7 @@
       <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -17205,70 +16792,70 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -17293,7 +16880,7 @@
       <selection pane="bottomRight" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -18526,98 +18113,98 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="22">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F7:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V7:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V7:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -18635,10 +18222,10 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="N52" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
       <selection pane="bottomRight" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -20649,74 +20236,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I10 I12:I54" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I10 I12:I54" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -20734,10 +20321,10 @@
   <dimension ref="B1:AD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
       <selection pane="bottomRight" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -21890,74 +21477,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I10 I12:I30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I10 I12:I30" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -21974,7 +21561,7 @@
   </sheetPr>
   <dimension ref="B1:AD30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -23141,74 +22728,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U30" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R31:U48" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -25280,74 +24867,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J19 J24:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J19 J24:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -25365,10 +24952,10 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
       <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -27423,74 +27010,74 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J19 J24:J54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J10 J12:J19 J24:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K10 K12:K19 K24:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F10 F12:F19 F24:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H10 H12:H19 H24:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:U54" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R55:U72" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
sync at start/end of exp., progress messages to Slack w/spreadsheets
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -3298,9 +3298,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
+      <xdr:colOff>88200</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3309,8 +3309,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3368880" y="10725120"/>
-          <a:ext cx="6655320" cy="2253600"/>
+          <a:off x="3369600" y="10725120"/>
+          <a:ext cx="6655680" cy="2253240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3557,9 +3557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1112400</xdr:colOff>
+      <xdr:colOff>1112040</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3573,7 +3573,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10722600"/>
-          <a:ext cx="3160080" cy="3269520"/>
+          <a:ext cx="3160440" cy="3269160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3599,9 +3599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
+      <xdr:colOff>66240</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3610,8 +3610,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3346920" y="7834680"/>
-          <a:ext cx="6655320" cy="2253600"/>
+          <a:off x="3347640" y="7834680"/>
+          <a:ext cx="6655680" cy="2253240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3858,9 +3858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1156320</xdr:colOff>
+      <xdr:colOff>1155960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3874,7 +3874,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7716240"/>
-          <a:ext cx="3204000" cy="1828080"/>
+          <a:ext cx="3204360" cy="1827720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3900,9 +3900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1728000</xdr:colOff>
+      <xdr:colOff>1727640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3911,8 +3911,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3401640" y="13656600"/>
-          <a:ext cx="6655320" cy="2253600"/>
+          <a:off x="3402360" y="13656600"/>
+          <a:ext cx="6655680" cy="2253240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4159,9 +4159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1146960</xdr:colOff>
+      <xdr:colOff>1146600</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4175,7 +4175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="158040" y="13629240"/>
-          <a:ext cx="3036600" cy="3112200"/>
+          <a:ext cx="3036960" cy="3111840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4201,9 +4201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>321840</xdr:colOff>
+      <xdr:colOff>321480</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4217,7 +4217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7947360"/>
-          <a:ext cx="3597480" cy="2252160"/>
+          <a:ext cx="3598560" cy="2251800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4238,14 +4238,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1321200</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865160</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:colOff>1864800</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4255,7 +4255,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648120" cy="2253600"/>
+          <a:ext cx="6647760" cy="2253240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4493,43 +4493,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112400</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="10262880"/>
-          <a:ext cx="3153240" cy="3269520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4544,621 +4507,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1865160</xdr:colOff>
+      <xdr:colOff>1864800</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648120" cy="2253600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="73080">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Instructions:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>2. Default values for all parameters go in line 6</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Specify detector position in column U, blank means to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>not move</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t> the detector </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Do not add rows above row 7</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>7. Do not add columns before column AE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112400</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5659920"/>
-          <a:ext cx="3153240" cy="3269520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1321200</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1865160</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648120" cy="2253600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="73080">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Instructions:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>2. Default values for all parameters go in line 6</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Specify detector position in column U, blank means to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>not move</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t> the detector </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>6. Do not add rows above row 7</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>7. Do not add columns before column AE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1112400</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5659920"/>
-          <a:ext cx="3153240" cy="3269520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1321200</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1606680</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6648120" cy="2253600"/>
+          <a:ext cx="6647760" cy="2253240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5413,14 +4774,14 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M2" activeCellId="1" sqref="I50:J53 M2"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7705,11 +7066,11 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="I50" activeCellId="0" sqref="I50:J53"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="I50" activeCellId="0" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9966,8 +9327,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9978,11 +9338,11 @@
   </sheetPr>
   <dimension ref="B1:AD80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D67" activeCellId="1" sqref="I50:J53 D67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -13297,10 +12657,10 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I50:J53 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -13438,10 +12798,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N22" activeCellId="1" sqref="I50:J53 N22"/>
+      <selection pane="bottomRight" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -14768,14 +14128,14 @@
   <dimension ref="B1:AF54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="1" sqref="I50:J53 F7"/>
+      <selection pane="bottomLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -17143,14 +16503,14 @@
   <dimension ref="B1:AE30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F10" activeCellId="1" sqref="I50:J53 F10"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -18492,11 +17852,11 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="N25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E19" activeCellId="1" sqref="I50:J53 E19"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20578,8 +19938,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20591,11 +19950,11 @@
   <dimension ref="B1:AD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F29" activeCellId="1" sqref="I50:J53 F29"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21836,7 +21195,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L12" activeCellId="1" sqref="I50:J53 L12"/>
+      <selection pane="bottomRight" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23083,11 +22442,11 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="E54" activeCellId="1" sqref="I50:J53 E54"/>
+      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25221,11 +24580,11 @@
   <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="1" sqref="I50:J53 I8"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
a list of small changes
+ use socket in dossier.py to determine host BS is running on
+ temporarily comment out disfunctional USB2 camera
+ a stab at wiggling mirrors before changing edge, currently commented out
+ specify a retraction distance for GA macro builder
+ carefully initialize 3 motor positions for grid macro
+ remove troublesome characters from filenames in spreadsheets
+ change_edge a bit more verbose
+ try harder (but still imperfectly) to get bender killed after moving
+ remove unneeded xspress3_ophyd_debug.log
+ comment out use of mpl_multitab in consumer
</commit_message>
<xml_diff>
--- a/startup/standards/standards.xlsx
+++ b/startup/standards/standards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Fe" sheetId="1" state="visible" r:id="rId2"/>
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="555">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -1441,6 +1441,15 @@
   </si>
   <si>
     <t xml:space="preserve">CuS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuCl2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CuCl2, eriochalcite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample coutesy Ankita Mohanty and Karen Chen-Wiegart, Stony Brook</t>
   </si>
   <si>
     <t xml:space="preserve">Znfoil</t>
@@ -3411,9 +3420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>86760</xdr:colOff>
+      <xdr:colOff>86400</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>51840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3422,8 +3431,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3372840" y="10725120"/>
-          <a:ext cx="6657120" cy="2251800"/>
+          <a:off x="3374280" y="10725120"/>
+          <a:ext cx="6657840" cy="2251440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3670,9 +3679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1110600</xdr:colOff>
+      <xdr:colOff>1110240</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3686,7 +3695,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="10722600"/>
-          <a:ext cx="3162240" cy="3267720"/>
+          <a:ext cx="3162960" cy="3267360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3712,9 +3721,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3723,8 +3732,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3350880" y="7834680"/>
-          <a:ext cx="6657120" cy="2251800"/>
+          <a:off x="3352320" y="7834680"/>
+          <a:ext cx="6657840" cy="2251440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3971,9 +3980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1154520</xdr:colOff>
+      <xdr:colOff>1154160</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3987,7 +3996,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7716240"/>
-          <a:ext cx="3206160" cy="1826280"/>
+          <a:ext cx="3206880" cy="1825920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4013,9 +4022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1726200</xdr:colOff>
+      <xdr:colOff>1725840</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4024,8 +4033,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3405600" y="13656600"/>
-          <a:ext cx="6657480" cy="2251800"/>
+          <a:off x="3407040" y="13656600"/>
+          <a:ext cx="6658200" cy="2251440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4272,9 +4281,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1145160</xdr:colOff>
+      <xdr:colOff>1144800</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4288,7 +4297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="158040" y="13771080"/>
-          <a:ext cx="3038760" cy="3110400"/>
+          <a:ext cx="3039480" cy="3110040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4314,9 +4323,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:colOff>319680</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4330,7 +4339,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7947360"/>
-          <a:ext cx="3601440" cy="2250360"/>
+          <a:ext cx="3602520" cy="2250000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4356,9 +4365,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1863360</xdr:colOff>
+      <xdr:colOff>1863000</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4368,7 +4377,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6646320" cy="2251800"/>
+          <a:ext cx="6645960" cy="2251440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4620,9 +4629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1863360</xdr:colOff>
+      <xdr:colOff>1863000</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4632,7 +4641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362040" y="10725120"/>
-          <a:ext cx="6646320" cy="2251800"/>
+          <a:ext cx="6645960" cy="2251440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4894,7 +4903,7 @@
       <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -7460,7 +7469,7 @@
         <v>49</v>
       </c>
       <c r="I6" s="112" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J6" s="113" t="s">
         <v>51</v>
@@ -7562,18 +7571,18 @@
         <v>5</v>
       </c>
       <c r="E8" s="129" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F8" s="89"/>
       <c r="G8" s="89"/>
       <c r="H8" s="89"/>
       <c r="I8" s="130" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J8" s="131"/>
       <c r="K8" s="126"/>
       <c r="L8" s="132" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="M8" s="129"/>
       <c r="N8" s="61" t="s">
@@ -7603,18 +7612,18 @@
         <v>5</v>
       </c>
       <c r="E9" s="107" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F9" s="89"/>
       <c r="G9" s="89"/>
       <c r="H9" s="89"/>
       <c r="I9" s="130" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J9" s="131"/>
       <c r="K9" s="126"/>
       <c r="L9" s="132" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="M9" s="129"/>
       <c r="N9" s="61" t="s">
@@ -7644,18 +7653,18 @@
         <v>5</v>
       </c>
       <c r="E10" s="107" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F10" s="89"/>
       <c r="G10" s="89"/>
       <c r="H10" s="89"/>
       <c r="I10" s="130" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J10" s="131"/>
       <c r="K10" s="126"/>
       <c r="L10" s="132" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="M10" s="129"/>
       <c r="N10" s="61" t="s">
@@ -7685,24 +7694,24 @@
         <v>5</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
       <c r="I11" s="130" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="132" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="M11" s="129" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="N11" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O11" s="0"/>
       <c r="P11" s="107"/>
@@ -8223,18 +8232,18 @@
         <v>5</v>
       </c>
       <c r="E27" s="107" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="F27" s="89"/>
       <c r="G27" s="89"/>
       <c r="H27" s="89"/>
       <c r="I27" s="130" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J27" s="131"/>
       <c r="K27" s="126"/>
       <c r="L27" s="132" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="M27" s="129"/>
       <c r="N27" s="61" t="s">
@@ -8264,18 +8273,18 @@
         <v>5</v>
       </c>
       <c r="E28" s="107" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="F28" s="89"/>
       <c r="G28" s="89"/>
       <c r="H28" s="89"/>
       <c r="I28" s="130" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J28" s="131"/>
       <c r="K28" s="126"/>
       <c r="L28" s="132" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="M28" s="129"/>
       <c r="N28" s="61" t="s">
@@ -8305,18 +8314,18 @@
         <v>5</v>
       </c>
       <c r="E29" s="107" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="F29" s="89"/>
       <c r="G29" s="89"/>
       <c r="H29" s="89"/>
       <c r="I29" s="130" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J29" s="131"/>
       <c r="K29" s="126"/>
       <c r="L29" s="132" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M29" s="107"/>
       <c r="N29" s="61" t="s">
@@ -8346,18 +8355,18 @@
         <v>5</v>
       </c>
       <c r="E30" s="107" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="F30" s="89"/>
       <c r="G30" s="89"/>
       <c r="H30" s="89"/>
       <c r="I30" s="130" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J30" s="131"/>
       <c r="K30" s="126"/>
       <c r="L30" s="132" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="M30" s="107"/>
       <c r="N30" s="61" t="s">
@@ -8453,18 +8462,18 @@
         <v>5</v>
       </c>
       <c r="E33" s="107" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F33" s="89"/>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>
       <c r="I33" s="130" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="J33" s="131"/>
       <c r="K33" s="126"/>
       <c r="L33" s="132" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="M33" s="129"/>
       <c r="N33" s="61" t="s">
@@ -9020,18 +9029,18 @@
         <v>5</v>
       </c>
       <c r="E50" s="107" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F50" s="89"/>
       <c r="G50" s="89"/>
       <c r="H50" s="89"/>
       <c r="I50" s="130" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J50" s="131"/>
       <c r="K50" s="126"/>
       <c r="L50" s="132" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="M50" s="129"/>
       <c r="N50" s="61" t="s">
@@ -9061,24 +9070,24 @@
         <v>5</v>
       </c>
       <c r="E51" s="107" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F51" s="89"/>
       <c r="G51" s="89"/>
       <c r="H51" s="89"/>
       <c r="I51" s="130" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J51" s="131"/>
       <c r="K51" s="126"/>
       <c r="L51" s="132" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="M51" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N51" s="133" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="O51" s="132"/>
       <c r="P51" s="107"/>
@@ -9104,24 +9113,24 @@
         <v>5</v>
       </c>
       <c r="E52" s="107" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F52" s="89"/>
       <c r="G52" s="89"/>
       <c r="H52" s="89"/>
       <c r="I52" s="130" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J52" s="131"/>
       <c r="K52" s="126"/>
       <c r="L52" s="132" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="M52" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N52" s="133" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="O52" s="132"/>
       <c r="P52" s="107"/>
@@ -9147,18 +9156,18 @@
         <v>5</v>
       </c>
       <c r="E53" s="107" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="F53" s="89"/>
       <c r="G53" s="89"/>
       <c r="H53" s="89"/>
       <c r="I53" s="130" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J53" s="131"/>
       <c r="K53" s="126"/>
       <c r="L53" s="132" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="M53" s="107"/>
       <c r="N53" s="61" t="s">
@@ -9188,24 +9197,24 @@
         <v>5</v>
       </c>
       <c r="E54" s="107" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="F54" s="89"/>
       <c r="G54" s="89"/>
       <c r="H54" s="89"/>
       <c r="I54" s="130" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J54" s="131"/>
       <c r="K54" s="126"/>
       <c r="L54" s="132" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="M54" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N54" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O54" s="132"/>
       <c r="P54" s="107"/>
@@ -9602,7 +9611,7 @@
         <v>49</v>
       </c>
       <c r="I6" s="112" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J6" s="113" t="s">
         <v>135</v>
@@ -9617,7 +9626,7 @@
         <v>294</v>
       </c>
       <c r="N6" s="117" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="O6" s="118" t="s">
         <v>56</v>
@@ -9704,26 +9713,26 @@
         <v>5</v>
       </c>
       <c r="E8" s="129" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F8" s="89"/>
       <c r="G8" s="89"/>
       <c r="H8" s="89"/>
       <c r="I8" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J8" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K8" s="126"/>
       <c r="L8" s="129" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="M8" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N8" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O8" s="132"/>
       <c r="P8" s="107"/>
@@ -9749,20 +9758,20 @@
         <v>5</v>
       </c>
       <c r="E9" s="107" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F9" s="89"/>
       <c r="G9" s="89"/>
       <c r="H9" s="89"/>
       <c r="I9" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J9" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K9" s="126"/>
       <c r="L9" s="107" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="M9" s="129"/>
       <c r="N9" s="61" t="s">
@@ -9792,26 +9801,26 @@
         <v>5</v>
       </c>
       <c r="E10" s="107" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F10" s="89"/>
       <c r="G10" s="89"/>
       <c r="H10" s="89"/>
       <c r="I10" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J10" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K10" s="126"/>
       <c r="L10" s="107" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="M10" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N10" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O10" s="132"/>
       <c r="P10" s="107"/>
@@ -9837,26 +9846,26 @@
         <v>5</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
       <c r="I11" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J11" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K11" s="0"/>
       <c r="L11" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="M11" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N11" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O11" s="132"/>
       <c r="P11" s="107"/>
@@ -9882,26 +9891,26 @@
         <v>5</v>
       </c>
       <c r="E12" s="107" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="F12" s="89"/>
       <c r="G12" s="89"/>
       <c r="H12" s="89"/>
       <c r="I12" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J12" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K12" s="126"/>
       <c r="L12" s="132" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="M12" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N12" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O12" s="132"/>
       <c r="P12" s="107"/>
@@ -9927,26 +9936,26 @@
         <v>5</v>
       </c>
       <c r="E13" s="107" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F13" s="89"/>
       <c r="G13" s="89"/>
       <c r="H13" s="89"/>
       <c r="I13" s="130" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J13" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K13" s="126"/>
       <c r="L13" s="132" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="M13" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N13" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O13" s="132"/>
       <c r="P13" s="107"/>
@@ -10401,26 +10410,26 @@
         <v>5</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
       <c r="I27" s="130" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J27" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K27" s="0"/>
       <c r="L27" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="M27" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N27" s="61" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O27" s="132"/>
       <c r="P27" s="107"/>
@@ -10446,26 +10455,26 @@
         <v>5</v>
       </c>
       <c r="E28" s="107" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="F28" s="89"/>
       <c r="G28" s="89"/>
       <c r="H28" s="89"/>
       <c r="I28" s="130" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J28" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K28" s="126"/>
       <c r="L28" s="143" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="M28" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N28" s="133" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="O28" s="132"/>
       <c r="P28" s="107"/>
@@ -10491,26 +10500,26 @@
         <v>5</v>
       </c>
       <c r="E29" s="107" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F29" s="89"/>
       <c r="G29" s="89"/>
       <c r="H29" s="89"/>
       <c r="I29" s="130" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J29" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K29" s="126"/>
       <c r="L29" s="132" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="M29" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N29" s="133" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="O29" s="132"/>
       <c r="P29" s="107"/>
@@ -10536,26 +10545,26 @@
         <v>5</v>
       </c>
       <c r="E30" s="107" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F30" s="89"/>
       <c r="G30" s="89"/>
       <c r="H30" s="89"/>
       <c r="I30" s="130" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J30" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K30" s="126"/>
       <c r="L30" s="107" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="M30" s="129" t="s">
         <v>54</v>
       </c>
       <c r="N30" s="133" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="O30" s="132"/>
       <c r="P30" s="107"/>
@@ -10614,20 +10623,20 @@
         <v>5</v>
       </c>
       <c r="E32" s="129" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="F32" s="89"/>
       <c r="G32" s="89"/>
       <c r="H32" s="89"/>
       <c r="I32" s="130" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J32" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K32" s="126"/>
       <c r="L32" s="132" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="M32" s="129"/>
       <c r="N32" s="61" t="s">
@@ -10657,20 +10666,20 @@
         <v>5</v>
       </c>
       <c r="E33" s="107" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="F33" s="89"/>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>
       <c r="I33" s="130" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J33" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K33" s="126"/>
       <c r="L33" s="132" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="M33" s="129" t="s">
         <v>54</v>
@@ -10899,20 +10908,20 @@
         <v>5</v>
       </c>
       <c r="E40" s="107" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F40" s="89"/>
       <c r="G40" s="89"/>
       <c r="H40" s="89"/>
       <c r="I40" s="130" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J40" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K40" s="126"/>
       <c r="L40" s="132" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="M40" s="129" t="s">
         <v>54</v>
@@ -10942,20 +10951,20 @@
         <v>5</v>
       </c>
       <c r="E41" s="107" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F41" s="89"/>
       <c r="G41" s="89"/>
       <c r="H41" s="89"/>
       <c r="I41" s="130" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J41" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K41" s="126"/>
       <c r="L41" s="132" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="M41" s="129" t="s">
         <v>54</v>
@@ -10985,20 +10994,20 @@
         <v>5</v>
       </c>
       <c r="E42" s="107" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="F42" s="89"/>
       <c r="G42" s="89"/>
       <c r="H42" s="89"/>
       <c r="I42" s="130" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J42" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K42" s="126"/>
       <c r="L42" s="132" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="M42" s="129" t="s">
         <v>54</v>
@@ -11028,20 +11037,20 @@
         <v>5</v>
       </c>
       <c r="E43" s="107" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F43" s="89"/>
       <c r="G43" s="89"/>
       <c r="H43" s="89"/>
       <c r="I43" s="130" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J43" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K43" s="126"/>
       <c r="L43" s="132" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="M43" s="129" t="s">
         <v>54</v>
@@ -11170,20 +11179,20 @@
         <v>5</v>
       </c>
       <c r="E47" s="107" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="F47" s="89"/>
       <c r="G47" s="89"/>
       <c r="H47" s="89"/>
       <c r="I47" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J47" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K47" s="126"/>
       <c r="L47" s="132" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="M47" s="129" t="s">
         <v>54</v>
@@ -11213,23 +11222,23 @@
         <v>5</v>
       </c>
       <c r="E48" s="107" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="F48" s="89"/>
       <c r="G48" s="89"/>
       <c r="H48" s="89"/>
       <c r="I48" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J48" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K48" s="126"/>
       <c r="L48" s="143" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="M48" s="129" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="N48" s="133"/>
       <c r="O48" s="132"/>
@@ -11289,23 +11298,23 @@
         <v>5</v>
       </c>
       <c r="E50" s="107" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F50" s="89"/>
       <c r="G50" s="89"/>
       <c r="H50" s="89"/>
       <c r="I50" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J50" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K50" s="126"/>
       <c r="L50" s="132" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="M50" s="129" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="N50" s="133"/>
       <c r="O50" s="132"/>
@@ -11332,23 +11341,23 @@
         <v>5</v>
       </c>
       <c r="E51" s="107" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="F51" s="89"/>
       <c r="G51" s="89"/>
       <c r="H51" s="89"/>
       <c r="I51" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J51" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K51" s="126"/>
       <c r="L51" s="132" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="M51" s="129" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="N51" s="133"/>
       <c r="O51" s="132"/>
@@ -11375,24 +11384,24 @@
         <v>5</v>
       </c>
       <c r="E52" s="107" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="F52" s="89"/>
       <c r="G52" s="89"/>
       <c r="H52" s="89"/>
       <c r="I52" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J52" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K52" s="126"/>
       <c r="L52" s="107" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="M52" s="129"/>
       <c r="N52" s="61" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="O52" s="132"/>
       <c r="P52" s="107"/>
@@ -11418,20 +11427,20 @@
         <v>5</v>
       </c>
       <c r="E53" s="107" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="F53" s="89"/>
       <c r="G53" s="89"/>
       <c r="H53" s="89"/>
       <c r="I53" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J53" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K53" s="126"/>
       <c r="L53" s="132" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="M53" s="107"/>
       <c r="N53" s="61" t="s">
@@ -11461,20 +11470,20 @@
         <v>5</v>
       </c>
       <c r="E54" s="107" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="F54" s="89"/>
       <c r="G54" s="89"/>
       <c r="H54" s="89"/>
       <c r="I54" s="130" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J54" s="131" t="s">
         <v>135</v>
       </c>
       <c r="K54" s="126"/>
       <c r="L54" s="132" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="M54" s="129"/>
       <c r="N54" s="61" t="s">
@@ -11597,7 +11606,7 @@
       <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -11876,7 +11885,7 @@
         <v>227</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>51</v>
@@ -11945,26 +11954,26 @@
         <v>5</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="151" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="J7" s="152" t="s">
         <v>51</v>
       </c>
       <c r="K7" s="48"/>
       <c r="L7" s="54" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="M7" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N7" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O7" s="54"/>
       <c r="P7" s="29"/>
@@ -11990,20 +11999,20 @@
         <v>5</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="151" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="J8" s="152" t="s">
         <v>135</v>
       </c>
       <c r="K8" s="48"/>
       <c r="L8" s="54" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="M8" s="51" t="s">
         <v>77</v>
@@ -12012,7 +12021,7 @@
         <v>140</v>
       </c>
       <c r="O8" s="64" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="55"/>
@@ -12037,20 +12046,20 @@
         <v>3</v>
       </c>
       <c r="E9" s="157" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="F9" s="154"/>
       <c r="G9" s="154"/>
       <c r="H9" s="154"/>
       <c r="I9" s="158" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="J9" s="159" t="s">
         <v>135</v>
       </c>
       <c r="K9" s="154"/>
       <c r="L9" s="160" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="M9" s="157"/>
       <c r="N9" s="161"/>
@@ -12076,7 +12085,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -12095,7 +12104,7 @@
         <v>299</v>
       </c>
       <c r="N10" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O10" s="54"/>
       <c r="P10" s="29"/>
@@ -12121,7 +12130,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -12134,7 +12143,7 @@
       </c>
       <c r="K11" s="48"/>
       <c r="L11" s="54" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="M11" s="51" t="s">
         <v>77</v>
@@ -12143,7 +12152,7 @@
         <v>140</v>
       </c>
       <c r="O11" s="64" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="55"/>
@@ -12168,20 +12177,20 @@
         <v>5</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="151" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="J12" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K12" s="48"/>
       <c r="L12" s="54" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="M12" s="51" t="s">
         <v>77</v>
@@ -12213,7 +12222,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -12235,7 +12244,7 @@
         <v>140</v>
       </c>
       <c r="O13" s="64" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="55"/>
@@ -12260,7 +12269,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -12273,7 +12282,7 @@
       </c>
       <c r="K14" s="48"/>
       <c r="L14" s="54" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="M14" s="51" t="s">
         <v>77</v>
@@ -12307,26 +12316,26 @@
         <v>5</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="151" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="J15" s="152" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="54" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="M15" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N15" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O15" s="54"/>
       <c r="P15" s="29"/>
@@ -12352,20 +12361,20 @@
         <v>3</v>
       </c>
       <c r="E16" s="157" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="F16" s="154"/>
       <c r="G16" s="154"/>
       <c r="H16" s="154"/>
       <c r="I16" s="158" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="J16" s="159" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K16" s="154"/>
       <c r="L16" s="160" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="M16" s="157"/>
       <c r="N16" s="161"/>
@@ -12391,7 +12400,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -12404,7 +12413,7 @@
       </c>
       <c r="K17" s="48"/>
       <c r="L17" s="54" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="M17" s="51" t="s">
         <v>77</v>
@@ -12438,7 +12447,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -12447,11 +12456,11 @@
         <v>149</v>
       </c>
       <c r="J18" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="54" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="M18" s="51" t="s">
         <v>77</v>
@@ -12483,7 +12492,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -12496,13 +12505,13 @@
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="54" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="M19" s="51" t="s">
         <v>227</v>
       </c>
       <c r="N19" s="144" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="O19" s="54"/>
       <c r="P19" s="29"/>
@@ -12528,7 +12537,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -12537,7 +12546,7 @@
         <v>134</v>
       </c>
       <c r="J20" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="54" t="s">
@@ -12573,7 +12582,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="51" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -12586,7 +12595,7 @@
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="54" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="M21" s="51" t="s">
         <v>77</v>
@@ -12620,7 +12629,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -12629,11 +12638,11 @@
         <v>172</v>
       </c>
       <c r="J22" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="54" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="M22" s="51" t="s">
         <v>77</v>
@@ -12665,7 +12674,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -12678,7 +12687,7 @@
       </c>
       <c r="K23" s="48"/>
       <c r="L23" s="54" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="M23" s="51" t="s">
         <v>77</v>
@@ -12712,7 +12721,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="51" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -12725,13 +12734,13 @@
       </c>
       <c r="K24" s="48"/>
       <c r="L24" s="54" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="M24" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N24" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O24" s="54"/>
       <c r="P24" s="29"/>
@@ -12757,7 +12766,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -12766,11 +12775,11 @@
         <v>183</v>
       </c>
       <c r="J25" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K25" s="48"/>
       <c r="L25" s="54" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="M25" s="51" t="s">
         <v>77</v>
@@ -12802,7 +12811,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -12815,7 +12824,7 @@
       </c>
       <c r="K26" s="48"/>
       <c r="L26" s="54" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="M26" s="51" t="s">
         <v>77</v>
@@ -12849,7 +12858,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -12862,7 +12871,7 @@
       </c>
       <c r="K27" s="48"/>
       <c r="L27" s="54" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="M27" s="51" t="s">
         <v>77</v>
@@ -12896,7 +12905,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="51" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
@@ -12909,13 +12918,13 @@
       </c>
       <c r="K28" s="48"/>
       <c r="L28" s="54" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="M28" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N28" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O28" s="54"/>
       <c r="P28" s="29"/>
@@ -12941,7 +12950,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -12950,11 +12959,11 @@
         <v>151</v>
       </c>
       <c r="J29" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K29" s="48"/>
       <c r="L29" s="54" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="M29" s="51" t="s">
         <v>77</v>
@@ -12986,7 +12995,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -12999,7 +13008,7 @@
       </c>
       <c r="K30" s="48"/>
       <c r="L30" s="54" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="M30" s="51" t="s">
         <v>77</v>
@@ -13033,7 +13042,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -13042,11 +13051,11 @@
         <v>155</v>
       </c>
       <c r="J31" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K31" s="48"/>
       <c r="L31" s="54" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="M31" s="51" t="s">
         <v>77</v>
@@ -13078,7 +13087,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="51" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
@@ -13091,7 +13100,7 @@
       </c>
       <c r="K32" s="48"/>
       <c r="L32" s="54" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="M32" s="51" t="s">
         <v>77</v>
@@ -13125,7 +13134,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
@@ -13138,13 +13147,13 @@
       </c>
       <c r="K33" s="48"/>
       <c r="L33" s="54" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="M33" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N33" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O33" s="54"/>
       <c r="P33" s="29"/>
@@ -13170,7 +13179,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="51" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
@@ -13215,7 +13224,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="51" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
@@ -13224,11 +13233,11 @@
         <v>167</v>
       </c>
       <c r="J35" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K35" s="48"/>
       <c r="L35" s="54" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="M35" s="51" t="s">
         <v>77</v>
@@ -13260,7 +13269,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="51" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -13273,7 +13282,7 @@
       </c>
       <c r="K36" s="48"/>
       <c r="L36" s="54" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="M36" s="51" t="s">
         <v>77</v>
@@ -13305,7 +13314,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -13314,11 +13323,11 @@
         <v>189</v>
       </c>
       <c r="J37" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K37" s="48"/>
       <c r="L37" s="54" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="M37" s="51" t="s">
         <v>77</v>
@@ -13350,7 +13359,7 @@
         <v>5</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
@@ -13395,7 +13404,7 @@
         <v>5</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
@@ -13408,13 +13417,13 @@
       </c>
       <c r="K39" s="48"/>
       <c r="L39" s="54" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="M39" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N39" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O39" s="54"/>
       <c r="P39" s="29"/>
@@ -13440,7 +13449,7 @@
         <v>5</v>
       </c>
       <c r="E40" s="51" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -13449,11 +13458,11 @@
         <v>192</v>
       </c>
       <c r="J40" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K40" s="48"/>
       <c r="L40" s="54" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="M40" s="51" t="s">
         <v>77</v>
@@ -13485,7 +13494,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="51" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
@@ -13498,7 +13507,7 @@
       </c>
       <c r="K41" s="48"/>
       <c r="L41" s="54" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="M41" s="51" t="s">
         <v>77</v>
@@ -13530,7 +13539,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="51" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -13539,11 +13548,11 @@
         <v>195</v>
       </c>
       <c r="J42" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K42" s="48"/>
       <c r="L42" s="54" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="M42" s="51" t="s">
         <v>77</v>
@@ -13575,20 +13584,20 @@
         <v>5</v>
       </c>
       <c r="E43" s="51" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="151" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="J43" s="152" t="s">
         <v>135</v>
       </c>
       <c r="K43" s="48"/>
       <c r="L43" s="54" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="M43" s="51" t="s">
         <v>77</v>
@@ -13620,7 +13629,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="51" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -13633,13 +13642,13 @@
       </c>
       <c r="K44" s="48"/>
       <c r="L44" s="54" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="M44" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N44" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O44" s="54"/>
       <c r="P44" s="29"/>
@@ -13665,7 +13674,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="51" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -13674,7 +13683,7 @@
         <v>162</v>
       </c>
       <c r="J45" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K45" s="48"/>
       <c r="L45" s="54" t="s">
@@ -13710,20 +13719,20 @@
         <v>5</v>
       </c>
       <c r="E46" s="51" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="151" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="J46" s="152" t="s">
         <v>135</v>
       </c>
       <c r="K46" s="48"/>
       <c r="L46" s="54" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="M46" s="51" t="s">
         <v>77</v>
@@ -13755,7 +13764,7 @@
         <v>5</v>
       </c>
       <c r="E47" s="51" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -13764,11 +13773,11 @@
         <v>199</v>
       </c>
       <c r="J47" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K47" s="48"/>
       <c r="L47" s="54" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="M47" s="51" t="s">
         <v>77</v>
@@ -13800,20 +13809,20 @@
         <v>5</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="151" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="J48" s="152" t="s">
         <v>135</v>
       </c>
       <c r="K48" s="48"/>
       <c r="L48" s="54" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="M48" s="51" t="s">
         <v>77</v>
@@ -13845,20 +13854,20 @@
         <v>5</v>
       </c>
       <c r="E49" s="51" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="151" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="J49" s="152" t="s">
         <v>51</v>
       </c>
       <c r="K49" s="48"/>
       <c r="L49" s="54" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="M49" s="51" t="s">
         <v>77</v>
@@ -13890,7 +13899,7 @@
         <v>5</v>
       </c>
       <c r="E50" s="51" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -13899,7 +13908,7 @@
         <v>164</v>
       </c>
       <c r="J50" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K50" s="48"/>
       <c r="L50" s="54" t="s">
@@ -13935,20 +13944,20 @@
         <v>5</v>
       </c>
       <c r="E51" s="51" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
       <c r="I51" s="151" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J51" s="152" t="s">
         <v>135</v>
       </c>
       <c r="K51" s="48"/>
       <c r="L51" s="54" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="M51" s="144" t="s">
         <v>54</v>
@@ -13978,7 +13987,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -13987,11 +13996,11 @@
         <v>203</v>
       </c>
       <c r="J52" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K52" s="48"/>
       <c r="L52" s="54" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="M52" s="51" t="s">
         <v>77</v>
@@ -14023,20 +14032,20 @@
         <v>3</v>
       </c>
       <c r="E53" s="157" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="F53" s="154"/>
       <c r="G53" s="154"/>
       <c r="H53" s="154"/>
       <c r="I53" s="158" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="J53" s="159" t="s">
         <v>135</v>
       </c>
       <c r="K53" s="154"/>
       <c r="L53" s="160" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="M53" s="162"/>
       <c r="N53" s="161"/>
@@ -14062,20 +14071,20 @@
         <v>5</v>
       </c>
       <c r="E54" s="51" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="151" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="J54" s="152" t="s">
         <v>51</v>
       </c>
       <c r="K54" s="48"/>
       <c r="L54" s="54" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="M54" s="51" t="s">
         <v>77</v>
@@ -14107,16 +14116,16 @@
         <v>3</v>
       </c>
       <c r="E55" s="157" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="I55" s="158" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="J55" s="159" t="s">
         <v>135</v>
       </c>
       <c r="L55" s="153" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="N55" s="164"/>
       <c r="V55" s="165"/>
@@ -14137,16 +14146,16 @@
         <v>5</v>
       </c>
       <c r="E56" s="51" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="I56" s="151" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="J56" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L56" s="54" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="M56" s="51" t="s">
         <v>77</v>
@@ -14166,22 +14175,22 @@
         <v>5</v>
       </c>
       <c r="E57" s="51" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="I57" s="151" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J57" s="152" t="s">
         <v>135</v>
       </c>
       <c r="L57" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="M57" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N57" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14195,16 +14204,16 @@
         <v>5</v>
       </c>
       <c r="E58" s="51" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="I58" s="151" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="J58" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L58" s="54" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="M58" s="51" t="s">
         <v>77</v>
@@ -14224,16 +14233,16 @@
         <v>5</v>
       </c>
       <c r="E59" s="51" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I59" s="151" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="J59" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="M59" s="144" t="s">
         <v>54</v>
@@ -14250,22 +14259,22 @@
         <v>5</v>
       </c>
       <c r="E60" s="51" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="I60" s="151" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J60" s="152" t="s">
         <v>135</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="M60" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N60" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14279,16 +14288,16 @@
         <v>5</v>
       </c>
       <c r="E61" s="51" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="I61" s="151" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="J61" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L61" s="54" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="M61" s="51" t="s">
         <v>77</v>
@@ -14308,16 +14317,16 @@
         <v>5</v>
       </c>
       <c r="E62" s="51" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="I62" s="151" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="J62" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L62" s="54" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="M62" s="144" t="s">
         <v>54</v>
@@ -14334,16 +14343,16 @@
         <v>5</v>
       </c>
       <c r="E63" s="51" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="I63" s="151" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="J63" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L63" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="M63" s="51" t="s">
         <v>77</v>
@@ -14363,16 +14372,16 @@
         <v>3</v>
       </c>
       <c r="E64" s="157" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="I64" s="158" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="J64" s="159" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L64" s="160" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="N64" s="164"/>
       <c r="V64" s="165"/>
@@ -14393,22 +14402,22 @@
         <v>5</v>
       </c>
       <c r="E65" s="51" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="I65" s="151" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J65" s="152" t="s">
         <v>135</v>
       </c>
       <c r="L65" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="M65" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N65" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14422,16 +14431,16 @@
         <v>5</v>
       </c>
       <c r="E66" s="51" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="I66" s="151" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J66" s="152" t="s">
         <v>135</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="M66" s="144" t="s">
         <v>54</v>
@@ -14449,16 +14458,16 @@
         <v>3</v>
       </c>
       <c r="E67" s="157" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="I67" s="158" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="J67" s="159" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L67" s="153" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="N67" s="164"/>
       <c r="V67" s="165"/>
@@ -14479,22 +14488,22 @@
         <v>5</v>
       </c>
       <c r="E68" s="51" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="I68" s="151" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="J68" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L68" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="M68" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="N68" s="61" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14508,16 +14517,16 @@
         <v>5</v>
       </c>
       <c r="E69" s="51" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="I69" s="151" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="J69" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L69" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="M69" s="51" t="s">
         <v>299</v>
@@ -14534,16 +14543,16 @@
         <v>5</v>
       </c>
       <c r="E70" s="51" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="I70" s="151" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J70" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="M70" s="51" t="s">
         <v>299</v>
@@ -14560,16 +14569,16 @@
         <v>5</v>
       </c>
       <c r="E71" s="51" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="I71" s="151" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="J71" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="M71" s="51" t="s">
         <v>77</v>
@@ -14589,22 +14598,22 @@
         <v>5</v>
       </c>
       <c r="E72" s="51" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="I72" s="151" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J72" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="M72" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N72" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14618,7 +14627,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="51" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="I73" s="151" t="s">
         <v>232</v>
@@ -14647,16 +14656,16 @@
         <v>5</v>
       </c>
       <c r="E74" s="51" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="I74" s="151" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J74" s="152" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="L74" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="M74" s="144" t="s">
         <v>54</v>
@@ -14673,16 +14682,16 @@
         <v>5</v>
       </c>
       <c r="E75" s="51" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="I75" s="151" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="J75" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="M75" s="51" t="s">
         <v>77</v>
@@ -14702,22 +14711,22 @@
         <v>5</v>
       </c>
       <c r="E76" s="51" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="I76" s="151" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="J76" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L76" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="M76" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N76" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14731,22 +14740,22 @@
         <v>5</v>
       </c>
       <c r="E77" s="51" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="I77" s="151" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="J77" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L77" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="M77" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N77" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14760,22 +14769,22 @@
         <v>5</v>
       </c>
       <c r="E78" s="51" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="I78" s="151" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J78" s="152" t="s">
         <v>51</v>
       </c>
       <c r="L78" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="M78" s="51" t="s">
         <v>299</v>
       </c>
       <c r="N78" s="144" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="79" s="166" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14789,16 +14798,16 @@
         <v>3</v>
       </c>
       <c r="E79" s="170" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="I79" s="171" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="J79" s="172" t="s">
         <v>51</v>
       </c>
       <c r="L79" s="166" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="M79" s="173" t="s">
         <v>77</v>
@@ -14915,7 +14924,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -14923,12 +14932,12 @@
   <sheetData>
     <row r="1" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B2" s="177"/>
     </row>
@@ -14944,10 +14953,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B5" s="177" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14955,7 +14964,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14963,7 +14972,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14971,7 +14980,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14979,7 +14988,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14987,7 +14996,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14995,7 +15004,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15003,7 +15012,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15011,7 +15020,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15019,7 +15028,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15027,7 +15036,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -15056,7 +15065,7 @@
       <selection pane="bottomRight" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -16382,7 +16391,7 @@
   </sheetPr>
   <dimension ref="B1:AF54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -16390,7 +16399,7 @@
       <selection pane="bottomRight" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -18775,7 +18784,7 @@
       <selection pane="bottomRight" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -24706,12 +24715,12 @@
   </sheetPr>
   <dimension ref="B1:AD54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25255,7 +25264,7 @@
       <c r="AA11" s="137"/>
       <c r="AB11" s="138"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="126" t="n">
         <v>6</v>
       </c>
@@ -25263,18 +25272,28 @@
         <v>46</v>
       </c>
       <c r="D12" s="128" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="107"/>
+        <v>5</v>
+      </c>
+      <c r="E12" s="107" t="s">
+        <v>306</v>
+      </c>
       <c r="F12" s="89"/>
       <c r="G12" s="89"/>
       <c r="H12" s="89"/>
-      <c r="I12" s="130"/>
+      <c r="I12" s="130" t="s">
+        <v>296</v>
+      </c>
       <c r="J12" s="131"/>
       <c r="K12" s="126"/>
-      <c r="L12" s="132"/>
-      <c r="M12" s="129"/>
-      <c r="N12" s="133"/>
+      <c r="L12" s="132" t="s">
+        <v>307</v>
+      </c>
+      <c r="M12" s="129" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="133" t="s">
+        <v>308</v>
+      </c>
       <c r="O12" s="132"/>
       <c r="P12" s="107"/>
       <c r="Q12" s="134"/>
@@ -25497,7 +25516,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="107" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F19" s="89"/>
       <c r="G19" s="89"/>
@@ -25510,7 +25529,7 @@
       <c r="J19" s="131"/>
       <c r="K19" s="126"/>
       <c r="L19" s="132" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="M19" s="129" t="s">
         <v>298</v>
@@ -25542,7 +25561,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
@@ -25553,7 +25572,7 @@
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
       <c r="L20" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="M20" s="0"/>
       <c r="N20" s="61" t="s">
@@ -25583,7 +25602,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
@@ -25594,7 +25613,7 @@
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
       <c r="L21" s="143" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="M21" s="0"/>
       <c r="N21" s="61" t="s">
@@ -25624,7 +25643,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
@@ -25635,7 +25654,7 @@
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
       <c r="L22" s="143" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="M22" s="0"/>
       <c r="N22" s="61" t="s">
@@ -25665,7 +25684,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
@@ -25676,7 +25695,7 @@
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
       <c r="L23" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="M23" s="0"/>
       <c r="N23" s="61" t="s">
@@ -25706,7 +25725,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="107" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F24" s="89"/>
       <c r="G24" s="89"/>
@@ -25719,7 +25738,7 @@
       <c r="J24" s="131"/>
       <c r="K24" s="126"/>
       <c r="L24" s="132" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="M24" s="129"/>
       <c r="N24" s="61" t="s">
@@ -25751,7 +25770,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="107" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F25" s="89"/>
       <c r="G25" s="89"/>
@@ -25762,7 +25781,7 @@
       <c r="J25" s="131"/>
       <c r="K25" s="126"/>
       <c r="L25" s="143" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="M25" s="129"/>
       <c r="N25" s="61" t="s">
@@ -27126,7 +27145,7 @@
         <v>49</v>
       </c>
       <c r="I6" s="112" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="J6" s="113" t="s">
         <v>51</v>
@@ -27228,7 +27247,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="107" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="F8" s="89"/>
       <c r="G8" s="89"/>
@@ -27237,11 +27256,11 @@
       <c r="J8" s="131"/>
       <c r="K8" s="126"/>
       <c r="L8" s="143" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="M8" s="129"/>
       <c r="N8" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O8" s="132"/>
       <c r="P8" s="107"/>
@@ -27267,7 +27286,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="107" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="F9" s="89"/>
       <c r="G9" s="89"/>
@@ -27276,11 +27295,11 @@
       <c r="J9" s="131"/>
       <c r="K9" s="126"/>
       <c r="L9" s="132" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="M9" s="129"/>
       <c r="N9" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O9" s="132"/>
       <c r="P9" s="107"/>
@@ -27306,7 +27325,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -27315,11 +27334,11 @@
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="M10" s="0"/>
       <c r="N10" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O10" s="132"/>
       <c r="P10" s="107"/>
@@ -27345,7 +27364,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -27354,11 +27373,11 @@
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="143" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="M11" s="0"/>
       <c r="N11" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O11" s="132"/>
       <c r="P11" s="107"/>
@@ -27384,7 +27403,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -27393,11 +27412,11 @@
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
       <c r="L12" s="143" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="M12" s="0"/>
       <c r="N12" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O12" s="132"/>
       <c r="P12" s="107"/>
@@ -27423,7 +27442,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -27432,11 +27451,11 @@
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
       <c r="L13" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="M13" s="0"/>
       <c r="N13" s="61" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="O13" s="132"/>
       <c r="P13" s="107"/>
@@ -27462,7 +27481,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F14" s="89"/>
       <c r="G14" s="89"/>
@@ -27471,11 +27490,11 @@
       <c r="J14" s="131"/>
       <c r="K14" s="126"/>
       <c r="L14" s="132" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="M14" s="129"/>
       <c r="N14" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O14" s="132"/>
       <c r="P14" s="107"/>
@@ -27501,7 +27520,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F15" s="89"/>
       <c r="G15" s="89"/>
@@ -27510,11 +27529,11 @@
       <c r="J15" s="131"/>
       <c r="K15" s="126"/>
       <c r="L15" s="143" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="M15" s="129"/>
       <c r="N15" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O15" s="132"/>
       <c r="P15" s="107"/>
@@ -27540,7 +27559,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="107" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F16" s="89"/>
       <c r="G16" s="89"/>
@@ -27549,11 +27568,11 @@
       <c r="J16" s="131"/>
       <c r="K16" s="126"/>
       <c r="L16" s="107" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="M16" s="129"/>
       <c r="N16" s="61" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="O16" s="132"/>
       <c r="P16" s="107"/>
@@ -27579,7 +27598,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="107" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F17" s="89"/>
       <c r="G17" s="89"/>
@@ -27588,7 +27607,7 @@
       <c r="J17" s="131"/>
       <c r="K17" s="126"/>
       <c r="L17" s="132" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="M17" s="129"/>
       <c r="N17" s="133"/>
@@ -27682,18 +27701,18 @@
         <v>5</v>
       </c>
       <c r="E20" s="75" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F20" s="89"/>
       <c r="G20" s="89"/>
       <c r="H20" s="89"/>
       <c r="I20" s="130" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="J20" s="131"/>
       <c r="K20" s="126"/>
       <c r="L20" s="107" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="M20" s="129"/>
       <c r="N20" s="61" t="s">

</xml_diff>